<commit_message>
Added Status Report Pdfs
</commit_message>
<xml_diff>
--- a/Status Reports/MiniGreen - Week 7 - Project Status Report.xlsx
+++ b/Status Reports/MiniGreen - Week 7 - Project Status Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21705"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\001427082\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronhebert/OneDrive - New England Institute of Technology/Senior Project/Status Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="11_2A3B567F1379B5E3FECDFA7F0E5CAA61B3B43953" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{24D20326-E33C-4200-AD5C-F42364FCADEA}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="11_2A3B567F1379B5E3FECDFA7F0E5CAA61B3B43953" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{08C4FA76-3D49-8249-9E7C-45153A101B06}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="440" windowWidth="25520" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -870,54 +870,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection sqref="A1:D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" customWidth="1"/>
+    <col min="2" max="2" width="42.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="31.5">
+    <row r="1" spans="2:4" ht="31">
       <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="26"/>
       <c r="D1" s="26"/>
     </row>
-    <row r="3" spans="2:4" ht="31.5">
+    <row r="3" spans="2:4" ht="31">
       <c r="B3" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="26"/>
     </row>
-    <row r="5" spans="2:4" ht="24" thickBot="1">
+    <row r="5" spans="2:4" ht="25" thickBot="1">
       <c r="B5" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="28"/>
       <c r="D5" s="28"/>
     </row>
-    <row r="6" spans="2:4" ht="27.75" thickBot="1">
+    <row r="6" spans="2:4" ht="30" thickBot="1">
       <c r="B6" s="29" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="31"/>
     </row>
-    <row r="7" spans="2:4" ht="31.5">
+    <row r="7" spans="2:4" ht="31">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="2:4" ht="24" thickBot="1">
+    <row r="8" spans="2:4" ht="25" thickBot="1">
       <c r="B8" s="27" t="s">
         <v>4</v>
       </c>
@@ -943,12 +946,12 @@
       <c r="C11" s="20"/>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="2:4" ht="15.75" thickBot="1">
+    <row r="12" spans="2:4" ht="16" thickBot="1">
       <c r="B12" s="22"/>
       <c r="C12" s="23"/>
       <c r="D12" s="24"/>
     </row>
-    <row r="14" spans="2:4" ht="24" thickBot="1">
+    <row r="14" spans="2:4" ht="25" thickBot="1">
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -980,7 +983,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="15.75" thickBot="1">
+    <row r="18" spans="2:4" ht="16" thickBot="1">
       <c r="B18" s="10" t="s">
         <v>12</v>
       </c>
@@ -989,7 +992,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="24" thickBot="1">
+    <row r="20" spans="2:4" ht="25" thickBot="1">
       <c r="B20" s="3" t="s">
         <v>14</v>
       </c>
@@ -1016,7 +1019,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="15.75" thickBot="1">
+    <row r="23" spans="2:4" ht="16" thickBot="1">
       <c r="B23" s="10" t="s">
         <v>18</v>
       </c>
@@ -1025,7 +1028,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="24" thickBot="1">
+    <row r="25" spans="2:4" ht="25" thickBot="1">
       <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
@@ -1036,7 +1039,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="15.75" thickBot="1">
+    <row r="26" spans="2:4" ht="16" thickBot="1">
       <c r="B26" s="16" t="s">
         <v>22</v>
       </c>
@@ -1047,7 +1050,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="24" thickBot="1">
+    <row r="28" spans="2:4" ht="25" thickBot="1">
       <c r="B28" s="3" t="s">
         <v>25</v>
       </c>
@@ -1074,7 +1077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="15.75" thickBot="1">
+    <row r="31" spans="2:4" ht="16" thickBot="1">
       <c r="B31" s="10" t="s">
         <v>29</v>
       </c>
@@ -1083,7 +1086,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="24" thickBot="1">
+    <row r="33" spans="2:4" ht="25" thickBot="1">
       <c r="B33" s="3" t="s">
         <v>30</v>
       </c>
@@ -1106,12 +1109,12 @@
       <c r="C35" s="2"/>
       <c r="D35" s="9"/>
     </row>
-    <row r="36" spans="2:4" ht="15.75" thickBot="1">
+    <row r="36" spans="2:4" ht="16" thickBot="1">
       <c r="B36" s="10"/>
       <c r="C36" s="11"/>
       <c r="D36" s="12"/>
     </row>
-    <row r="38" spans="2:4" ht="24" thickBot="1">
+    <row r="38" spans="2:4" ht="25" thickBot="1">
       <c r="B38" s="3" t="s">
         <v>34</v>
       </c>
@@ -1130,12 +1133,12 @@
       <c r="C40" s="2"/>
       <c r="D40" s="14"/>
     </row>
-    <row r="41" spans="2:4" ht="15.75" thickBot="1">
+    <row r="41" spans="2:4" ht="16" thickBot="1">
       <c r="B41" s="10"/>
       <c r="C41" s="11"/>
       <c r="D41" s="15"/>
     </row>
-    <row r="43" spans="2:4" ht="24" thickBot="1">
+    <row r="43" spans="2:4" ht="25" thickBot="1">
       <c r="B43" s="3" t="s">
         <v>35</v>
       </c>
@@ -1154,12 +1157,12 @@
       <c r="C45" s="2"/>
       <c r="D45" s="14"/>
     </row>
-    <row r="46" spans="2:4" ht="15.75" thickBot="1">
+    <row r="46" spans="2:4" ht="16" thickBot="1">
       <c r="B46" s="10"/>
       <c r="C46" s="11"/>
       <c r="D46" s="15"/>
     </row>
-    <row r="48" spans="2:4" ht="24" thickBot="1">
+    <row r="48" spans="2:4" ht="25" thickBot="1">
       <c r="B48" s="3" t="s">
         <v>37</v>
       </c>
@@ -1182,7 +1185,7 @@
       <c r="C50" s="2"/>
       <c r="D50" s="9"/>
     </row>
-    <row r="51" spans="2:4" ht="15.75" thickBot="1">
+    <row r="51" spans="2:4" ht="16" thickBot="1">
       <c r="B51" s="10"/>
       <c r="C51" s="11"/>
       <c r="D51" s="12"/>
@@ -1200,5 +1203,6 @@
     <mergeCell ref="B9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="73" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>